<commit_message>
Added the night background into the object value spreadsheet
</commit_message>
<xml_diff>
--- a/SMB1/Research Docs/Object Values.xlsx
+++ b/SMB1/Research Docs/Object Values.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="274">
   <si>
     <t>Y Offset 0x0 - 0xB</t>
   </si>
@@ -909,37 +908,22 @@
   </si>
   <si>
     <t>Nothing</t>
+  </si>
+  <si>
+    <t>Change Background: Night</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -951,7 +935,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -959,198 +943,458 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3214285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.8877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.5612244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.0510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.6683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="42.280612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="13" style="0" width="22.6224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.7959183673469"/>
+    <col min="1" max="1" width="16.21875"/>
+    <col min="2" max="2" width="42.5546875"/>
+    <col min="3" max="3" width="26.21875"/>
+    <col min="4" max="4" width="28"/>
+    <col min="5" max="5" width="28.33203125"/>
+    <col min="6" max="6" width="29.88671875"/>
+    <col min="7" max="7" width="31.5546875"/>
+    <col min="8" max="8" width="39"/>
+    <col min="9" max="9" width="26.21875"/>
+    <col min="10" max="10" width="31.6640625"/>
+    <col min="11" max="11" width="42.21875"/>
+    <col min="12" max="12" width="24.33203125"/>
+    <col min="13" max="17" width="22.6640625"/>
+    <col min="18" max="1025" width="11.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="N3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1196,1338 +1440,1338 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="L5" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M5" t="s">
         <v>60</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="N5" t="s">
         <v>61</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="O5" t="s">
         <v>62</v>
       </c>
-      <c r="P5" s="0" t="s">
+      <c r="P5" t="s">
         <v>63</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" t="s">
         <v>58</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="L6" t="s">
         <v>59</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M6" t="s">
         <v>60</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="N6" t="s">
         <v>61</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="O6" t="s">
         <v>62</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="P6" t="s">
         <v>63</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" t="s">
         <v>58</v>
       </c>
-      <c r="L7" s="0" t="s">
+      <c r="L7" t="s">
         <v>59</v>
       </c>
-      <c r="M7" s="0" t="s">
+      <c r="M7" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="0" t="s">
+      <c r="N7" t="s">
         <v>61</v>
       </c>
-      <c r="O7" s="0" t="s">
+      <c r="O7" t="s">
         <v>62</v>
       </c>
-      <c r="P7" s="0" t="s">
+      <c r="P7" t="s">
         <v>63</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" t="s">
         <v>58</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="L8" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="M8" t="s">
         <v>60</v>
       </c>
-      <c r="N8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="N8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" t="s">
         <v>58</v>
       </c>
-      <c r="L9" s="0" t="s">
+      <c r="L9" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="0" t="s">
+      <c r="M9" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q9" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="N9" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="K10" t="s">
         <v>83</v>
       </c>
-      <c r="L10" s="0" t="s">
+      <c r="L10" t="s">
         <v>84</v>
       </c>
-      <c r="M10" s="0" t="s">
+      <c r="M10" t="s">
         <v>85</v>
       </c>
-      <c r="N10" s="0" t="s">
+      <c r="N10" t="s">
         <v>86</v>
       </c>
-      <c r="O10" s="0" t="s">
+      <c r="O10" t="s">
         <v>87</v>
       </c>
-      <c r="P10" s="0" t="s">
+      <c r="P10" t="s">
         <v>88</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="K13" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="0" t="s">
+      <c r="L13" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="0" t="s">
+      <c r="M13" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="0" t="s">
+      <c r="N13" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="0" t="s">
+      <c r="O13" t="s">
         <v>14</v>
       </c>
-      <c r="P13" s="0" t="s">
+      <c r="P13" t="s">
         <v>15</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="Q13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" t="s">
         <v>56</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="J14" t="s">
         <v>57</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="K14" t="s">
         <v>58</v>
       </c>
-      <c r="L14" s="0" t="s">
+      <c r="L14" t="s">
         <v>59</v>
       </c>
-      <c r="M14" s="0" t="s">
+      <c r="M14" t="s">
         <v>60</v>
       </c>
-      <c r="N14" s="0" t="s">
+      <c r="N14" t="s">
         <v>61</v>
       </c>
-      <c r="O14" s="0" t="s">
+      <c r="O14" t="s">
         <v>62</v>
       </c>
-      <c r="P14" s="0" t="s">
+      <c r="P14" t="s">
         <v>63</v>
       </c>
-      <c r="Q14" s="0" t="s">
+      <c r="Q14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" t="s">
         <v>56</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" t="s">
         <v>57</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="K15" t="s">
         <v>58</v>
       </c>
-      <c r="L15" s="0" t="s">
+      <c r="L15" t="s">
         <v>59</v>
       </c>
-      <c r="M15" s="0" t="s">
+      <c r="M15" t="s">
         <v>60</v>
       </c>
-      <c r="N15" s="0" t="s">
+      <c r="N15" t="s">
         <v>61</v>
       </c>
-      <c r="O15" s="0" t="s">
+      <c r="O15" t="s">
         <v>62</v>
       </c>
-      <c r="P15" s="0" t="s">
+      <c r="P15" t="s">
         <v>63</v>
       </c>
-      <c r="Q15" s="0" t="s">
+      <c r="Q15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" t="s">
         <v>56</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="J16" t="s">
         <v>57</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="K16" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="0" t="s">
+      <c r="L16" t="s">
         <v>59</v>
       </c>
-      <c r="M16" s="0" t="s">
+      <c r="M16" t="s">
         <v>60</v>
       </c>
-      <c r="N16" s="0" t="s">
+      <c r="N16" t="s">
         <v>61</v>
       </c>
-      <c r="O16" s="0" t="s">
+      <c r="O16" t="s">
         <v>62</v>
       </c>
-      <c r="P16" s="0" t="s">
+      <c r="P16" t="s">
         <v>63</v>
       </c>
-      <c r="Q16" s="0" t="s">
+      <c r="Q16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="G17" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" t="s">
         <v>56</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="J17" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="K17" t="s">
         <v>58</v>
       </c>
-      <c r="L17" s="0" t="s">
+      <c r="L17" t="s">
         <v>59</v>
       </c>
-      <c r="M17" s="0" t="s">
+      <c r="M17" t="s">
         <v>60</v>
       </c>
-      <c r="N17" s="0" t="s">
+      <c r="N17" t="s">
         <v>61</v>
       </c>
-      <c r="O17" s="0" t="s">
+      <c r="O17" t="s">
         <v>62</v>
       </c>
-      <c r="P17" s="0" t="s">
+      <c r="P17" t="s">
         <v>63</v>
       </c>
-      <c r="Q17" s="0" t="s">
+      <c r="Q17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" t="s">
         <v>56</v>
       </c>
-      <c r="J18" s="0" t="s">
+      <c r="J18" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="0" t="s">
+      <c r="K18" t="s">
         <v>58</v>
       </c>
-      <c r="L18" s="0" t="s">
+      <c r="L18" t="s">
         <v>59</v>
       </c>
-      <c r="M18" s="0" t="s">
+      <c r="M18" t="s">
         <v>60</v>
       </c>
-      <c r="N18" s="0" t="s">
+      <c r="N18" t="s">
         <v>61</v>
       </c>
-      <c r="O18" s="0" t="s">
+      <c r="O18" t="s">
         <v>62</v>
       </c>
-      <c r="P18" s="0" t="s">
+      <c r="P18" t="s">
         <v>63</v>
       </c>
-      <c r="Q18" s="0" t="s">
+      <c r="Q18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="0" t="s">
+      <c r="J19" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="0" t="s">
+      <c r="K19" t="s">
         <v>58</v>
       </c>
-      <c r="L19" s="0" t="s">
+      <c r="L19" t="s">
         <v>59</v>
       </c>
-      <c r="M19" s="0" t="s">
+      <c r="M19" t="s">
         <v>60</v>
       </c>
-      <c r="N19" s="0" t="s">
+      <c r="N19" t="s">
         <v>61</v>
       </c>
-      <c r="O19" s="0" t="s">
+      <c r="O19" t="s">
         <v>62</v>
       </c>
-      <c r="P19" s="0" t="s">
+      <c r="P19" t="s">
         <v>63</v>
       </c>
-      <c r="Q19" s="0" t="s">
+      <c r="Q19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="G20" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="H20" t="s">
         <v>55</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="J20" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="K20" t="s">
         <v>58</v>
       </c>
-      <c r="L20" s="0" t="s">
+      <c r="L20" t="s">
         <v>59</v>
       </c>
-      <c r="M20" s="0" t="s">
+      <c r="M20" t="s">
         <v>60</v>
       </c>
-      <c r="N20" s="0" t="s">
+      <c r="N20" t="s">
         <v>61</v>
       </c>
-      <c r="O20" s="0" t="s">
+      <c r="O20" t="s">
         <v>62</v>
       </c>
-      <c r="P20" s="0" t="s">
+      <c r="P20" t="s">
         <v>63</v>
       </c>
-      <c r="Q20" s="0" t="s">
+      <c r="Q20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G21" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" t="s">
         <v>57</v>
       </c>
-      <c r="K21" s="0" t="s">
+      <c r="K21" t="s">
         <v>58</v>
       </c>
-      <c r="L21" s="0" t="s">
+      <c r="L21" t="s">
         <v>59</v>
       </c>
-      <c r="M21" s="0" t="s">
+      <c r="M21" t="s">
         <v>60</v>
       </c>
-      <c r="N21" s="0" t="s">
+      <c r="N21" t="s">
         <v>61</v>
       </c>
-      <c r="O21" s="0" t="s">
+      <c r="O21" t="s">
         <v>62</v>
       </c>
-      <c r="P21" s="0" t="s">
+      <c r="P21" t="s">
         <v>63</v>
       </c>
-      <c r="Q21" s="0" t="s">
+      <c r="Q21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="H24" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="0" t="s">
+      <c r="J24" t="s">
         <v>9</v>
       </c>
-      <c r="K24" s="0" t="s">
+      <c r="K24" t="s">
         <v>10</v>
       </c>
-      <c r="L24" s="0" t="s">
+      <c r="L24" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="0" t="s">
+      <c r="M24" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="0" t="s">
+      <c r="N24" t="s">
         <v>13</v>
       </c>
-      <c r="O24" s="0" t="s">
+      <c r="O24" t="s">
         <v>14</v>
       </c>
-      <c r="P24" s="0" t="s">
+      <c r="P24" t="s">
         <v>15</v>
       </c>
-      <c r="Q24" s="0" t="s">
+      <c r="Q24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="G25" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="H25" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="I25" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="0" t="s">
+      <c r="J25" t="s">
         <v>56</v>
       </c>
-      <c r="K25" s="0" t="s">
+      <c r="K25" t="s">
         <v>57</v>
       </c>
-      <c r="L25" s="0" t="s">
+      <c r="L25" t="s">
         <v>58</v>
       </c>
-      <c r="M25" s="0" t="s">
+      <c r="M25" t="s">
         <v>59</v>
       </c>
-      <c r="N25" s="0" t="s">
+      <c r="N25" t="s">
         <v>60</v>
       </c>
-      <c r="O25" s="0" t="s">
+      <c r="O25" t="s">
         <v>61</v>
       </c>
-      <c r="P25" s="0" t="s">
+      <c r="P25" t="s">
         <v>62</v>
       </c>
-      <c r="Q25" s="0" t="s">
+      <c r="Q25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="G26" t="s">
         <v>107</v>
       </c>
-      <c r="H26" s="0" t="s">
+      <c r="H26" t="s">
         <v>108</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I26" t="s">
         <v>109</v>
       </c>
-      <c r="J26" s="0" t="s">
+      <c r="J26" t="s">
         <v>110</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="K26" t="s">
         <v>111</v>
       </c>
-      <c r="L26" s="0" t="s">
+      <c r="L26" t="s">
         <v>112</v>
       </c>
-      <c r="M26" s="0" t="s">
+      <c r="M26" t="s">
         <v>113</v>
       </c>
-      <c r="N26" s="0" t="s">
+      <c r="N26" t="s">
         <v>114</v>
       </c>
-      <c r="O26" s="0" t="s">
+      <c r="O26" t="s">
         <v>115</v>
       </c>
-      <c r="P26" s="0" t="s">
+      <c r="P26" t="s">
         <v>116</v>
       </c>
-      <c r="Q26" s="0" t="s">
+      <c r="Q26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>118</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" t="s">
         <v>119</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" t="s">
         <v>120</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" t="s">
         <v>121</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" t="s">
         <v>122</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="G27" t="s">
         <v>123</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="H27" t="s">
         <v>124</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I27" t="s">
         <v>125</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="J27" t="s">
         <v>126</v>
       </c>
-      <c r="K27" s="0" t="s">
+      <c r="K27" t="s">
         <v>127</v>
       </c>
-      <c r="L27" s="0" t="s">
+      <c r="L27" t="s">
         <v>128</v>
       </c>
-      <c r="M27" s="0" t="s">
+      <c r="M27" t="s">
         <v>129</v>
       </c>
-      <c r="N27" s="0" t="s">
+      <c r="N27" t="s">
         <v>130</v>
       </c>
-      <c r="O27" s="0" t="s">
+      <c r="O27" t="s">
         <v>131</v>
       </c>
-      <c r="P27" s="0" t="s">
+      <c r="P27" t="s">
         <v>132</v>
       </c>
-      <c r="Q27" s="0" t="s">
+      <c r="Q27" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>134</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" t="s">
         <v>136</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" t="s">
         <v>137</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" t="s">
         <v>138</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="G28" t="s">
         <v>139</v>
       </c>
-      <c r="H28" s="0" t="s">
+      <c r="H28" t="s">
         <v>140</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="I28" t="s">
         <v>141</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="J28" t="s">
         <v>142</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="K28" t="s">
         <v>143</v>
       </c>
-      <c r="L28" s="0" t="s">
+      <c r="L28" t="s">
         <v>144</v>
       </c>
-      <c r="M28" s="0" t="s">
+      <c r="M28" t="s">
         <v>145</v>
       </c>
-      <c r="N28" s="0" t="s">
+      <c r="N28" t="s">
         <v>146</v>
       </c>
-      <c r="O28" s="0" t="s">
+      <c r="O28" t="s">
         <v>147</v>
       </c>
-      <c r="P28" s="0" t="s">
+      <c r="P28" t="s">
         <v>148</v>
       </c>
-      <c r="Q28" s="0" t="s">
+      <c r="Q28" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>150</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" t="s">
         <v>151</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" t="s">
         <v>152</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" t="s">
         <v>153</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" t="s">
         <v>154</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="G29" t="s">
         <v>155</v>
       </c>
-      <c r="H29" s="0" t="s">
+      <c r="H29" t="s">
         <v>156</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="I29" t="s">
         <v>156</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="J29" t="s">
         <v>157</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="K29" t="s">
         <v>158</v>
       </c>
-      <c r="L29" s="0" t="s">
+      <c r="L29" t="s">
         <v>159</v>
       </c>
-      <c r="M29" s="0" t="s">
+      <c r="M29" t="s">
         <v>160</v>
       </c>
-      <c r="N29" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O29" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P29" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q29" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="N29" t="s">
+        <v>30</v>
+      </c>
+      <c r="O29" t="s">
+        <v>30</v>
+      </c>
+      <c r="P29" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q30" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L30" t="s">
+        <v>30</v>
+      </c>
+      <c r="M30" t="s">
+        <v>30</v>
+      </c>
+      <c r="N30" t="s">
+        <v>30</v>
+      </c>
+      <c r="O30" t="s">
+        <v>30</v>
+      </c>
+      <c r="P30" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q31" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" t="s">
+        <v>30</v>
+      </c>
+      <c r="L31" t="s">
+        <v>30</v>
+      </c>
+      <c r="M31" t="s">
+        <v>30</v>
+      </c>
+      <c r="N31" t="s">
+        <v>30</v>
+      </c>
+      <c r="O31" t="s">
+        <v>30</v>
+      </c>
+      <c r="P31" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q32" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" t="s">
+        <v>30</v>
+      </c>
+      <c r="J32" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" t="s">
+        <v>30</v>
+      </c>
+      <c r="L32" t="s">
+        <v>30</v>
+      </c>
+      <c r="M32" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" t="s">
+        <v>30</v>
+      </c>
+      <c r="O32" t="s">
+        <v>30</v>
+      </c>
+      <c r="P32" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" t="s">
         <v>5</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="G35" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="H35" t="s">
         <v>7</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="I35" t="s">
         <v>8</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="J35" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="0" t="s">
+      <c r="K35" t="s">
         <v>10</v>
       </c>
-      <c r="L35" s="0" t="s">
+      <c r="L35" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="0" t="s">
+      <c r="M35" t="s">
         <v>12</v>
       </c>
-      <c r="N35" s="0" t="s">
+      <c r="N35" t="s">
         <v>13</v>
       </c>
-      <c r="O35" s="0" t="s">
+      <c r="O35" t="s">
         <v>14</v>
       </c>
-      <c r="P35" s="0" t="s">
+      <c r="P35" t="s">
         <v>15</v>
       </c>
-      <c r="Q35" s="0" t="s">
+      <c r="Q35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
@@ -2580,8 +2824,8 @@
         <v>177</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2633,8 +2877,8 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>48</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2686,8 +2930,8 @@
         <v>209</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>65</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2739,758 +2983,737 @@
         <v>225</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>226</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" t="s">
         <v>227</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" t="s">
         <v>228</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" t="s">
         <v>229</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G40" t="s">
         <v>230</v>
       </c>
-      <c r="G40" s="0" t="s">
+      <c r="H40" t="s">
         <v>231</v>
       </c>
-      <c r="H40" s="0" t="s">
+      <c r="I40" t="s">
         <v>232</v>
       </c>
-      <c r="I40" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J40" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K40" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L40" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M40" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N40" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O40" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P40" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q40" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="J40" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" t="s">
+        <v>30</v>
+      </c>
+      <c r="N40" t="s">
+        <v>30</v>
+      </c>
+      <c r="O40" t="s">
+        <v>30</v>
+      </c>
+      <c r="P40" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q41" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" t="s">
+        <v>30</v>
+      </c>
+      <c r="J41" t="s">
+        <v>30</v>
+      </c>
+      <c r="K41" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" t="s">
+        <v>30</v>
+      </c>
+      <c r="M41" t="s">
+        <v>30</v>
+      </c>
+      <c r="N41" t="s">
+        <v>30</v>
+      </c>
+      <c r="O41" t="s">
+        <v>30</v>
+      </c>
+      <c r="P41" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P42" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q42" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" t="s">
+        <v>30</v>
+      </c>
+      <c r="J42" t="s">
+        <v>30</v>
+      </c>
+      <c r="K42" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" t="s">
+        <v>30</v>
+      </c>
+      <c r="M42" t="s">
+        <v>30</v>
+      </c>
+      <c r="N42" t="s">
+        <v>30</v>
+      </c>
+      <c r="O42" t="s">
+        <v>30</v>
+      </c>
+      <c r="P42" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q43" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="B43" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" t="s">
+        <v>30</v>
+      </c>
+      <c r="J43" t="s">
+        <v>30</v>
+      </c>
+      <c r="K43" t="s">
+        <v>30</v>
+      </c>
+      <c r="L43" t="s">
+        <v>30</v>
+      </c>
+      <c r="M43" t="s">
+        <v>30</v>
+      </c>
+      <c r="N43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O43" t="s">
+        <v>30</v>
+      </c>
+      <c r="P43" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" t="s">
         <v>4</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="F46" t="s">
         <v>5</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="G46" t="s">
         <v>6</v>
       </c>
-      <c r="H46" s="0" t="s">
+      <c r="H46" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="0" t="s">
+      <c r="I46" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="0" t="s">
+      <c r="J46" t="s">
         <v>9</v>
       </c>
-      <c r="K46" s="0" t="s">
+      <c r="K46" t="s">
         <v>10</v>
       </c>
-      <c r="L46" s="0" t="s">
+      <c r="L46" t="s">
         <v>11</v>
       </c>
-      <c r="M46" s="0" t="s">
+      <c r="M46" t="s">
         <v>12</v>
       </c>
-      <c r="N46" s="0" t="s">
+      <c r="N46" t="s">
         <v>13</v>
       </c>
-      <c r="O46" s="0" t="s">
+      <c r="O46" t="s">
         <v>14</v>
       </c>
-      <c r="P46" s="0" t="s">
+      <c r="P46" t="s">
         <v>15</v>
       </c>
-      <c r="Q46" s="0" t="s">
+      <c r="Q46" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" t="s">
         <v>234</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P47" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q47" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" t="s">
+        <v>30</v>
+      </c>
+      <c r="I47" t="s">
+        <v>30</v>
+      </c>
+      <c r="J47" t="s">
+        <v>30</v>
+      </c>
+      <c r="K47" t="s">
+        <v>30</v>
+      </c>
+      <c r="L47" t="s">
+        <v>30</v>
+      </c>
+      <c r="M47" t="s">
+        <v>30</v>
+      </c>
+      <c r="N47" t="s">
+        <v>30</v>
+      </c>
+      <c r="O47" t="s">
+        <v>30</v>
+      </c>
+      <c r="P47" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" t="s">
         <v>235</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" t="s">
         <v>236</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" t="s">
         <v>237</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" t="s">
         <v>238</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="F48" t="s">
         <v>239</v>
       </c>
-      <c r="G48" s="0" t="s">
+      <c r="G48" t="s">
         <v>240</v>
       </c>
-      <c r="H48" s="0" t="s">
+      <c r="H48" t="s">
         <v>241</v>
       </c>
-      <c r="I48" s="0" t="s">
+      <c r="I48" t="s">
         <v>242</v>
       </c>
-      <c r="J48" s="0" t="s">
+      <c r="J48" t="s">
         <v>243</v>
       </c>
-      <c r="K48" s="0" t="s">
+      <c r="K48" t="s">
         <v>244</v>
       </c>
-      <c r="L48" s="0" t="s">
+      <c r="L48" t="s">
         <v>245</v>
       </c>
-      <c r="M48" s="0" t="s">
+      <c r="M48" t="s">
         <v>246</v>
       </c>
-      <c r="N48" s="0" t="s">
+      <c r="N48" t="s">
         <v>247</v>
       </c>
-      <c r="O48" s="0" t="s">
+      <c r="O48" t="s">
         <v>248</v>
       </c>
-      <c r="P48" s="0" t="s">
+      <c r="P48" t="s">
         <v>249</v>
       </c>
-      <c r="Q48" s="0" t="s">
+      <c r="Q48" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H49" s="0" t="s">
+      <c r="C49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" t="s">
         <v>252</v>
       </c>
-      <c r="I49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P49" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q49" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="I49" t="s">
+        <v>30</v>
+      </c>
+      <c r="J49" t="s">
+        <v>30</v>
+      </c>
+      <c r="K49" t="s">
+        <v>30</v>
+      </c>
+      <c r="L49" t="s">
+        <v>30</v>
+      </c>
+      <c r="M49" t="s">
+        <v>30</v>
+      </c>
+      <c r="N49" t="s">
+        <v>30</v>
+      </c>
+      <c r="O49" t="s">
+        <v>30</v>
+      </c>
+      <c r="P49" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>65</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" t="s">
         <v>253</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" t="s">
         <v>254</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" t="s">
         <v>255</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" t="s">
         <v>256</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="F50" t="s">
         <v>257</v>
       </c>
-      <c r="G50" s="0" t="s">
+      <c r="G50" t="s">
         <v>258</v>
       </c>
-      <c r="H50" s="0" t="s">
+      <c r="H50" t="s">
         <v>259</v>
       </c>
-      <c r="I50" s="0" t="s">
+      <c r="I50" t="s">
         <v>260</v>
       </c>
-      <c r="J50" s="0" t="s">
+      <c r="J50" t="s">
         <v>261</v>
       </c>
-      <c r="K50" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L50" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M50" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N50" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O50" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P50" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q50" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="K50" t="s">
+        <v>30</v>
+      </c>
+      <c r="L50" t="s">
+        <v>30</v>
+      </c>
+      <c r="M50" t="s">
+        <v>30</v>
+      </c>
+      <c r="N50" t="s">
+        <v>30</v>
+      </c>
+      <c r="O50" t="s">
+        <v>30</v>
+      </c>
+      <c r="P50" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="0" t="s">
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" t="s">
         <v>262</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" t="s">
         <v>263</v>
       </c>
-      <c r="F51" s="0" t="s">
+      <c r="F51" t="s">
         <v>264</v>
       </c>
-      <c r="G51" s="0" t="s">
+      <c r="G51" t="s">
         <v>265</v>
       </c>
-      <c r="H51" s="0" t="s">
+      <c r="H51" t="s">
         <v>266</v>
       </c>
-      <c r="I51" s="0" t="s">
+      <c r="I51" t="s">
         <v>267</v>
       </c>
-      <c r="J51" s="0" t="s">
+      <c r="J51" t="s">
         <v>268</v>
       </c>
-      <c r="K51" s="0" t="s">
+      <c r="K51" t="s">
         <v>269</v>
       </c>
-      <c r="L51" s="0" t="s">
+      <c r="L51" t="s">
         <v>270</v>
       </c>
-      <c r="M51" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N51" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O51" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P51" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q51" s="0" t="s">
+      <c r="M51" t="s">
+        <v>30</v>
+      </c>
+      <c r="N51" t="s">
+        <v>30</v>
+      </c>
+      <c r="O51" t="s">
+        <v>30</v>
+      </c>
+      <c r="P51" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q51" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P52" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q52" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="B52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" t="s">
+        <v>30</v>
+      </c>
+      <c r="H52" t="s">
+        <v>30</v>
+      </c>
+      <c r="I52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J52" t="s">
+        <v>30</v>
+      </c>
+      <c r="K52" t="s">
+        <v>30</v>
+      </c>
+      <c r="L52" t="s">
+        <v>30</v>
+      </c>
+      <c r="M52" t="s">
+        <v>30</v>
+      </c>
+      <c r="N52" t="s">
+        <v>30</v>
+      </c>
+      <c r="O52" t="s">
+        <v>30</v>
+      </c>
+      <c r="P52" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" t="s">
         <v>272</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q53" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="C53" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" t="s">
+        <v>30</v>
+      </c>
+      <c r="H53" t="s">
+        <v>30</v>
+      </c>
+      <c r="I53" t="s">
+        <v>30</v>
+      </c>
+      <c r="J53" t="s">
+        <v>30</v>
+      </c>
+      <c r="K53" t="s">
+        <v>30</v>
+      </c>
+      <c r="L53" t="s">
+        <v>30</v>
+      </c>
+      <c r="M53" t="s">
+        <v>30</v>
+      </c>
+      <c r="N53" t="s">
+        <v>30</v>
+      </c>
+      <c r="O53" t="s">
+        <v>30</v>
+      </c>
+      <c r="P53" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="N54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P54" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q54" s="0" t="s">
+      <c r="B54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I54" t="s">
+        <v>30</v>
+      </c>
+      <c r="J54" t="s">
+        <v>30</v>
+      </c>
+      <c r="K54" t="s">
+        <v>30</v>
+      </c>
+      <c r="L54" t="s">
+        <v>30</v>
+      </c>
+      <c r="M54" t="s">
+        <v>30</v>
+      </c>
+      <c r="N54" t="s">
+        <v>30</v>
+      </c>
+      <c r="O54" t="s">
+        <v>30</v>
+      </c>
+      <c r="P54" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q54" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.77734375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.77734375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>